<commit_message>
fixed README.md and history button
</commit_message>
<xml_diff>
--- a/tests/cahier_de_tests_calculatrice_Pierre.xlsx
+++ b/tests/cahier_de_tests_calculatrice_Pierre.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pierrot\Documents\HB_PharmaPilot\calculatrice\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pierrot\Documents\HB_PharmaPilot\calculatrice\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04038E16-DBAD-4BCE-97C2-0FB6D4BD20F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12A01B9B-8BB2-453F-9CE7-4CC195194971}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{B44055BC-57CB-4C0A-99E7-8C611C2DB950}"/>
   </bookViews>
@@ -98,13 +98,13 @@
     <t>division by 0</t>
   </si>
   <si>
-    <t>Add two integers 1 and 10 on the first entry and result appears in second entry</t>
-  </si>
-  <si>
-    <t>Add three integers 20, 30 and 50 on the first entry and result appears in second entry</t>
-  </si>
-  <si>
-    <t>Substract two floats 10.5 , .5 on the first entry and result appears in second entry</t>
+    <t>Add two integers 1 and 10 on the first entry and result appears in second line</t>
+  </si>
+  <si>
+    <t>Add three integers 20, 30 and 50 on the first entry</t>
+  </si>
+  <si>
+    <t>Substract two floats 10.5 , .5 on the first entry</t>
   </si>
 </sst>
 </file>
@@ -212,37 +212,37 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -258,12 +258,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B05828DD-E3D1-4EB7-9DB1-8789138CF034}" name="Tableau1" displayName="Tableau1" ref="A1:E11" totalsRowShown="0" dataDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B05828DD-E3D1-4EB7-9DB1-8789138CF034}" name="Tableau1" displayName="Tableau1" ref="A1:E11" totalsRowShown="0" dataDxfId="11">
   <autoFilter ref="A1:E11" xr:uid="{B05828DD-E3D1-4EB7-9DB1-8789138CF034}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{248BC16A-1685-488D-A22C-DE75AC3E58FC}" name="Scénario" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{40BCA765-9860-46C1-82C7-382A196E91A0}" name="Input" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{ABF3415F-136D-4AAE-902F-5C44E38562A5}" name="Résultat Attendu" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{248BC16A-1685-488D-A22C-DE75AC3E58FC}" name="Scénario" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{40BCA765-9860-46C1-82C7-382A196E91A0}" name="Input" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{ABF3415F-136D-4AAE-902F-5C44E38562A5}" name="Résultat Attendu" dataDxfId="8"/>
     <tableColumn id="4" xr3:uid="{A8083F3B-B067-4073-812E-52901A31CED7}" name="Résultat Obtenu" dataDxfId="7"/>
     <tableColumn id="5" xr3:uid="{DAB24C2A-38EC-4F3F-B562-B3615DFA512A}" name="Etat" dataDxfId="6"/>
   </tableColumns>
@@ -272,14 +272,14 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B46B2BCD-8D3F-47FF-A3FA-3C33A5E0E3DB}" name="Tableau2" displayName="Tableau2" ref="A1:E11" totalsRowShown="0" dataDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B46B2BCD-8D3F-47FF-A3FA-3C33A5E0E3DB}" name="Tableau2" displayName="Tableau2" ref="A1:E11" totalsRowShown="0" dataDxfId="5">
   <autoFilter ref="A1:E11" xr:uid="{B46B2BCD-8D3F-47FF-A3FA-3C33A5E0E3DB}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{D3C7E472-F328-47CD-906E-6E4C73AD5204}" name="Scénario" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{E110DA5D-E52E-4425-9798-4F767A5554E8}" name="Input" dataDxfId="0"/>
-    <tableColumn id="3" xr3:uid="{81CD7CD5-47D1-419D-B9F8-AD3EDD50B6C8}" name="Résultat Attendu" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{58B3EBD3-2BED-4F59-9C5F-C0E4092418F5}" name="Résultat Obtenu" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{3704C978-7EA5-4464-9EB0-037966868566}" name="Etat" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{D3C7E472-F328-47CD-906E-6E4C73AD5204}" name="Scénario" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{E110DA5D-E52E-4425-9798-4F767A5554E8}" name="Input" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{81CD7CD5-47D1-419D-B9F8-AD3EDD50B6C8}" name="Résultat Attendu" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{58B3EBD3-2BED-4F59-9C5F-C0E4092418F5}" name="Résultat Obtenu" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{3704C978-7EA5-4464-9EB0-037966868566}" name="Etat" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -585,7 +585,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -785,13 +785,13 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="68.33203125" customWidth="1"/>
-    <col min="2" max="2" width="28.44140625" customWidth="1"/>
+    <col min="1" max="1" width="63.77734375" customWidth="1"/>
+    <col min="2" max="2" width="22.88671875" customWidth="1"/>
     <col min="3" max="3" width="27" customWidth="1"/>
     <col min="4" max="4" width="26.77734375" customWidth="1"/>
     <col min="5" max="5" width="26" style="1" customWidth="1"/>

</xml_diff>